<commit_message>
added code in for redirect urls
</commit_message>
<xml_diff>
--- a/data/Buildings_Seperated_long_lat.xlsx
+++ b/data/Buildings_Seperated_long_lat.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\n_wol\OneDrive\Documents\GitHub\OswegoDashboardProject\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CEC158-8106-478B-B625-2E739495347C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAA6A95-8B6F-49DA-A5F3-CE421C28F640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="225">
   <si>
     <t>Cayuga Hall</t>
   </si>
@@ -686,423 +685,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>BLDG NO</t>
-  </si>
-  <si>
-    <t>BUILDING NAME</t>
-  </si>
-  <si>
-    <t>BLDG ABR GSF</t>
-  </si>
-  <si>
-    <t>SHELDON HALL</t>
-  </si>
-  <si>
-    <t>SLHL-1</t>
-  </si>
-  <si>
-    <t>J C PARK HALL</t>
-  </si>
-  <si>
-    <t>PKHL-2</t>
-  </si>
-  <si>
-    <t>CAMPUS CENTER</t>
-  </si>
-  <si>
-    <t>CC-3</t>
-  </si>
-  <si>
-    <t>M V LEE HALL</t>
-  </si>
-  <si>
-    <t>LEEPE4</t>
-  </si>
-  <si>
-    <t>SHADY SHORE</t>
-  </si>
-  <si>
-    <t>PRRES5</t>
-  </si>
-  <si>
-    <t>J LANIGAN HALL</t>
-  </si>
-  <si>
-    <t>LAN-6</t>
-  </si>
-  <si>
-    <t>J TYLER HALL</t>
-  </si>
-  <si>
-    <t>TYL-7</t>
-  </si>
-  <si>
-    <t>RICHARD S SHINEMAN CENTER</t>
-  </si>
-  <si>
-    <t>RSSC-8</t>
-  </si>
-  <si>
-    <t>WILBER HALL</t>
-  </si>
-  <si>
-    <t>WLR-9</t>
-  </si>
-  <si>
-    <t>MARY WALKER HEALTH CENTER</t>
-  </si>
-  <si>
-    <t>INF-10</t>
-  </si>
-  <si>
-    <t>COMMISSARY BLDG</t>
-  </si>
-  <si>
-    <t>COMS11</t>
-  </si>
-  <si>
-    <t>MAINTENANCE BLDG</t>
-  </si>
-  <si>
-    <t>MTCE12</t>
-  </si>
-  <si>
-    <t>M E MAHAR HALL</t>
-  </si>
-  <si>
-    <t>MAH-13</t>
-  </si>
-  <si>
-    <t>RICH HALL</t>
-  </si>
-  <si>
-    <t>RIC-14</t>
-  </si>
-  <si>
-    <t>MACKIN HALL</t>
-  </si>
-  <si>
-    <t>MKN-15</t>
-  </si>
-  <si>
-    <t>OBSERVATORY</t>
-  </si>
-  <si>
-    <t>OBS-16</t>
-  </si>
-  <si>
-    <t>J PENFIELD LIB</t>
-  </si>
-  <si>
-    <t>PLB-17</t>
-  </si>
-  <si>
-    <t>LAKER HALL</t>
-  </si>
-  <si>
-    <t>HPE-19</t>
-  </si>
-  <si>
-    <t>GAR-20</t>
-  </si>
-  <si>
-    <t>ROMNEY FIELD HSE</t>
-  </si>
-  <si>
-    <t>FLH-21</t>
-  </si>
-  <si>
-    <t>KING HALL</t>
-  </si>
-  <si>
-    <t>KG-22</t>
-  </si>
-  <si>
-    <t>CULKIN HALL</t>
-  </si>
-  <si>
-    <t>CUL-26</t>
-  </si>
-  <si>
-    <t>SEWAGE PUMP STATION</t>
-  </si>
-  <si>
-    <t>SEW-28</t>
-  </si>
-  <si>
-    <t>HEWITT HALL</t>
-  </si>
-  <si>
-    <t>HWT-29</t>
-  </si>
-  <si>
-    <t>PATHFINDER DH</t>
-  </si>
-  <si>
-    <t>PATH31</t>
-  </si>
-  <si>
-    <t>SENECA HALL</t>
-  </si>
-  <si>
-    <t>SEN-32</t>
-  </si>
-  <si>
-    <t>CAYUGA HALL</t>
-  </si>
-  <si>
-    <t>CAY-33</t>
-  </si>
-  <si>
-    <t>ONONDAGA HALL</t>
-  </si>
-  <si>
-    <t>ON-34</t>
-  </si>
-  <si>
-    <t>LITTLE PAGE DH</t>
-  </si>
-  <si>
-    <t>LIT-35</t>
-  </si>
-  <si>
-    <t>ONEIDA HALL</t>
-  </si>
-  <si>
-    <t>ODA-36</t>
-  </si>
-  <si>
-    <t>JOHNSON HALL</t>
-  </si>
-  <si>
-    <t>JNHL41</t>
-  </si>
-  <si>
-    <t>LAKESIDE DH</t>
-  </si>
-  <si>
-    <t>LKDN42</t>
-  </si>
-  <si>
-    <t>RIGGS HALL</t>
-  </si>
-  <si>
-    <t>RGH-43</t>
-  </si>
-  <si>
-    <t>WATERBURY HALL</t>
-  </si>
-  <si>
-    <t>WTB-44</t>
-  </si>
-  <si>
-    <t>SCALES HALL</t>
-  </si>
-  <si>
-    <t>SCL-45</t>
-  </si>
-  <si>
-    <t>HART HALL</t>
-  </si>
-  <si>
-    <t>HRT-46</t>
-  </si>
-  <si>
-    <t>COOPER DH</t>
-  </si>
-  <si>
-    <t>CPDN47</t>
-  </si>
-  <si>
-    <t>FUNNELLE HALL</t>
-  </si>
-  <si>
-    <t>FNL-48</t>
-  </si>
-  <si>
-    <t>PUBLIC RESTROOM</t>
-  </si>
-  <si>
-    <t>REST</t>
-  </si>
-  <si>
-    <t>FM RADIO TRANSMISSION FAC</t>
-  </si>
-  <si>
-    <t>TRNSM</t>
-  </si>
-  <si>
-    <t>METRO CENTER</t>
-  </si>
-  <si>
-    <t>METRO</t>
-  </si>
-  <si>
-    <t>MAINTENANCE STORAGE</t>
-  </si>
-  <si>
-    <t>STOR</t>
-  </si>
-  <si>
-    <t>POLE BARN</t>
-  </si>
-  <si>
-    <t>POL-1</t>
-  </si>
-  <si>
-    <t>FT DRM ED SVC CONSORTIUM</t>
-  </si>
-  <si>
-    <t>FTDRM</t>
-  </si>
-  <si>
-    <t>RICE CREEK OBSERVATORY</t>
-  </si>
-  <si>
-    <t>OBS-81</t>
-  </si>
-  <si>
-    <t>PRESS BOX</t>
-  </si>
-  <si>
-    <t>PRB-82</t>
-  </si>
-  <si>
-    <t>RICE CREEK PAVILION</t>
-  </si>
-  <si>
-    <t>RCP-83</t>
-  </si>
-  <si>
-    <t>BUSINESS AND COMMUNITY RELATIONS</t>
-  </si>
-  <si>
-    <t>BCR-84</t>
-  </si>
-  <si>
-    <t>BUSINESS RESOURCE CENTER</t>
-  </si>
-  <si>
-    <t>BRC-85</t>
-  </si>
-  <si>
-    <t>SECURITY PARKING OFFICE</t>
-  </si>
-  <si>
-    <t>CHS104</t>
-  </si>
-  <si>
-    <t>VOLATILE STO</t>
-  </si>
-  <si>
-    <t>PKHL2A</t>
-  </si>
-  <si>
-    <t>1 ROOM SCHOOL HSE</t>
-  </si>
-  <si>
-    <t>1RMSH</t>
-  </si>
-  <si>
-    <t>POWER STATION 1</t>
-  </si>
-  <si>
-    <t>PWR1</t>
-  </si>
-  <si>
-    <t>POWER STATION 1A</t>
-  </si>
-  <si>
-    <t>PWR1A</t>
-  </si>
-  <si>
-    <t>POWER STATION 2</t>
-  </si>
-  <si>
-    <t>PWR2</t>
-  </si>
-  <si>
-    <t>0003B</t>
-  </si>
-  <si>
-    <t>REC &amp; CONVOCATION CTR</t>
-  </si>
-  <si>
-    <t>CTR-3</t>
-  </si>
-  <si>
-    <t>0003C</t>
-  </si>
-  <si>
-    <t>CC STORAGE BLDG</t>
-  </si>
-  <si>
-    <t>CCSB</t>
-  </si>
-  <si>
-    <t>PRESIDENT GARAGE</t>
-  </si>
-  <si>
-    <t>PRRESG</t>
-  </si>
-  <si>
-    <t>0023A</t>
-  </si>
-  <si>
-    <t>RICE CREEK FIELD STATION</t>
-  </si>
-  <si>
-    <t>BIO23A</t>
-  </si>
-  <si>
-    <t>0024A</t>
-  </si>
-  <si>
-    <t>BIO FIELD GARAGE</t>
-  </si>
-  <si>
-    <t>BIO24A</t>
-  </si>
-  <si>
-    <t>SEWAGE PUMP STATION - SENECA</t>
-  </si>
-  <si>
-    <t>SEW28A</t>
-  </si>
-  <si>
-    <t>SEWAGE PUMP STATION - BLG 12</t>
-  </si>
-  <si>
-    <t>SEW28B</t>
-  </si>
-  <si>
-    <t>0037L</t>
-  </si>
-  <si>
-    <t>I POUCHER HALL</t>
-  </si>
-  <si>
-    <t>PO-3</t>
-  </si>
-  <si>
-    <t>LEE HALL (HEATING PLANT)</t>
-  </si>
-  <si>
-    <t>LEEHP4</t>
-  </si>
-  <si>
-    <t>MORELAND HALL</t>
-  </si>
-  <si>
-    <t>MRL15A</t>
-  </si>
-  <si>
-    <t>LONIS HALL</t>
-  </si>
-  <si>
-    <t>LNS15B</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -1119,16 +701,19 @@
   </si>
   <si>
     <t>squareFt</t>
+  </si>
+  <si>
+    <t>assetWorksPropertyUrl</t>
+  </si>
+  <si>
+    <t>https://aim.sucf.suny.edu/fmax/screen/MASTER_ASSET_VIEW?assetTag=1735</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0000"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1141,6 +726,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1161,10 +752,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1173,21 +765,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1404,10 +991,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G997"/>
+  <dimension ref="A1:I997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1416,33 +1003,38 @@
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="44.7109375" customWidth="1"/>
     <col min="5" max="6" width="41.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>357</v>
+        <v>218</v>
       </c>
       <c r="B1" t="s">
         <v>216</v>
       </c>
       <c r="C1" t="s">
-        <v>358</v>
+        <v>219</v>
       </c>
       <c r="D1" t="s">
-        <v>359</v>
+        <v>220</v>
       </c>
       <c r="E1" t="s">
         <v>215</v>
       </c>
       <c r="F1" t="s">
-        <v>360</v>
+        <v>221</v>
       </c>
       <c r="G1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
+        <v>222</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1459,8 +1051,8 @@
         <v>-76.507487999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1481,9 +1073,12 @@
       <c r="G3">
         <v>119211</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
+      <c r="I3" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1505,8 +1100,8 @@
         <v>66979</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1528,8 +1123,8 @@
         <v>185524</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1551,8 +1146,8 @@
         <v>65000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1574,8 +1169,8 @@
         <v>8754</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1597,8 +1192,8 @@
         <v>88200</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
+    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1620,8 +1215,8 @@
         <v>115430</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
+    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1643,8 +1238,8 @@
         <v>235860</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1666,8 +1261,8 @@
         <v>108933</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
+    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1689,8 +1284,8 @@
         <v>33260</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1712,8 +1307,8 @@
         <v>30836</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1735,8 +1330,8 @@
         <v>20664</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="8">
+    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1758,8 +1353,8 @@
         <v>91530</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
+    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1782,7 +1377,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="8">
+      <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1805,7 +1400,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="8">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1828,7 +1423,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="8">
+      <c r="A19" s="4">
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1851,7 +1446,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="8">
+      <c r="A20" s="4">
         <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1874,7 +1469,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="8">
+      <c r="A21" s="4">
         <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1897,7 +1492,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="8">
+      <c r="A22" s="4">
         <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1920,7 +1515,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="8">
+      <c r="A23" s="4">
         <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1939,11 +1534,11 @@
         <v>-76.550110628032797</v>
       </c>
       <c r="G23" t="s">
-        <v>356</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="8">
+      <c r="A24" s="4">
         <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1962,11 +1557,11 @@
         <v>-76.549306540607304</v>
       </c>
       <c r="G24" t="s">
-        <v>356</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="8">
+      <c r="A25" s="4">
         <v>26</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1989,7 +1584,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="8">
+      <c r="A26" s="4">
         <v>28</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -2012,7 +1607,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="8">
+      <c r="A27" s="4">
         <v>29</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -2035,7 +1630,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="8">
+      <c r="A28" s="4">
         <v>31</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -2058,7 +1653,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="8">
+      <c r="A29" s="4">
         <v>32</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2081,7 +1676,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="8">
+      <c r="A30" s="4">
         <v>33</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2104,7 +1699,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="8">
+      <c r="A31" s="4">
         <v>34</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -2127,7 +1722,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="8">
+      <c r="A32" s="4">
         <v>35</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2150,7 +1745,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="8">
+      <c r="A33" s="4">
         <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -2173,7 +1768,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="8">
+      <c r="A34" s="4">
         <v>41</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -2196,7 +1791,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="8">
+      <c r="A35" s="4">
         <v>42</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2219,7 +1814,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="8">
+      <c r="A36" s="4">
         <v>43</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -2242,7 +1837,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="8">
+      <c r="A37" s="4">
         <v>44</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2265,7 +1860,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="8">
+      <c r="A38" s="4">
         <v>45</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -2288,7 +1883,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="8">
+      <c r="A39" s="4">
         <v>46</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -2311,7 +1906,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="8">
+      <c r="A40" s="4">
         <v>47</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -2334,7 +1929,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="8">
+      <c r="A41" s="4">
         <v>48</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -2357,7 +1952,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="8">
+      <c r="A42" s="4">
         <v>53</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -2380,7 +1975,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="8">
+      <c r="A43" s="4">
         <v>71</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2403,7 +1998,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="8">
+      <c r="A44" s="4">
         <v>81</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -2426,7 +2021,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="8">
+      <c r="A45" s="4">
         <v>82</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -2449,7 +2044,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="8">
+      <c r="A46" s="4">
         <v>83</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -2472,7 +2067,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="8">
+      <c r="A47" s="4">
         <v>84</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -2495,7 +2090,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="8">
+      <c r="A48" s="4">
         <v>85</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -2518,7 +2113,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="8">
+      <c r="A49" s="4">
         <v>104</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -2541,7 +2136,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="8">
+      <c r="A50" s="4">
         <v>107</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -2951,7 +2546,7 @@
         <v>-76.542171055612002</v>
       </c>
       <c r="G67" t="s">
-        <v>356</v>
+        <v>217</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
@@ -2974,7 +2569,7 @@
         <v>-76.507127299999993</v>
       </c>
       <c r="G68" t="s">
-        <v>356</v>
+        <v>217</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
@@ -3066,7 +2661,7 @@
         <v>-76.542396545410099</v>
       </c>
       <c r="G72" t="s">
-        <v>356</v>
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
@@ -10473,1133 +10068,10 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H998">
     <sortCondition ref="A21:A998"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1" xr:uid="{4EAA15BE-A4D0-4A43-A361-5EA2E9946229}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4922470-3FD9-4BED-9430-684D5260C99A}">
-  <dimension ref="A1:D80"/>
-  <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="4" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="D2" s="5">
-        <v>119211</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" s="5">
-        <v>66979</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="D4" s="5">
-        <v>185524</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D5" s="5">
-        <v>65000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="D6" s="5">
-        <v>8754</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="D7" s="5">
-        <v>88200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>7</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="D8" s="5">
-        <v>115430</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="D9" s="5">
-        <v>235860</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="D10" s="5">
-        <v>108933</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="D11" s="5">
-        <v>33260</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="D12" s="5">
-        <v>30836</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="D13" s="5">
-        <v>20664</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D14" s="5">
-        <v>91530</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
-        <v>14</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D15" s="5">
-        <v>53742</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="D16" s="5">
-        <v>41984</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
-        <v>16</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="D17" s="5">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="D18" s="5">
-        <v>192298</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
-        <v>19</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="D19" s="5">
-        <v>196608</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
-        <v>20</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D20" s="5">
-        <v>14850</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
-        <v>21</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="D21" s="5">
-        <v>55000</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
-        <v>22</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="D22" s="5">
-        <v>7200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
-        <v>26</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="D23" s="5">
-        <v>63591</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
-        <v>28</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D24" s="5">
-        <v>1881</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
-        <v>29</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="D25" s="5">
-        <v>135010</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
-        <v>31</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="D26" s="5">
-        <v>33827</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
-        <v>32</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D27" s="5">
-        <v>152548</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="7">
-        <v>33</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="D28" s="5">
-        <v>105072</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="7">
-        <v>34</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="D29" s="5">
-        <v>152548</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="7">
-        <v>35</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="D30" s="5">
-        <v>33827</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
-        <v>36</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="D31" s="5">
-        <v>105000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
-        <v>41</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="D32" s="5">
-        <v>79097</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="7">
-        <v>42</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D33" s="5">
-        <v>27870</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="7">
-        <v>43</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D34" s="5">
-        <v>58201</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
-        <v>44</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="D35" s="5">
-        <v>57464</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
-        <v>45</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="D36" s="5">
-        <v>57464</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="7">
-        <v>46</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="D37" s="5">
-        <v>114365</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="7">
-        <v>47</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="D38" s="5">
-        <v>33546</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="7">
-        <v>48</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="D39" s="5">
-        <v>114365</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="7">
-        <v>49</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="D40" s="5">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="7">
-        <v>51</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="D41" s="5">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="7">
-        <v>53</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="D42" s="5">
-        <v>14526</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="7">
-        <v>61</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D43" s="5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="7">
-        <v>71</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="D44" s="5">
-        <v>6925</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="7">
-        <v>80</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="D45" s="5">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="7">
-        <v>81</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="D46" s="5">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="7">
-        <v>82</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="D47" s="5">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="7">
-        <v>83</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="D48" s="5">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="7">
-        <v>84</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="D49" s="5">
-        <v>1917</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="7">
-        <v>85</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="D50" s="5">
-        <v>2739</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="7">
-        <v>104</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="D51" s="5">
-        <v>2297</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="7">
-        <v>106</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="D52" s="5">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="7">
-        <v>107</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="D53" s="5">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="7">
-        <v>108</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="D54" s="5">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="7">
-        <v>109</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="D55" s="5">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="7">
-        <v>110</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="D56" s="5">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="D57" s="5">
-        <v>115421</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="D58" s="5">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="D59" s="5">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="D60" s="5">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
-        <v>340</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="D61" s="5">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="D62" s="5">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="D63" s="5">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D64" s="5">
-        <v>10260</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D65" s="5">
-        <v>8082</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D66" s="5">
-        <v>12599</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D67" s="5">
-        <v>12599</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D68" s="5">
-        <v>15880</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D69" s="5">
-        <v>18295</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D70" s="5">
-        <v>8082</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D71" s="5">
-        <v>10260</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D72" s="5">
-        <v>12599</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D73" s="5">
-        <v>12599</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D74" s="5">
-        <v>16729</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="6" t="s">
-        <v>347</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D75" s="5">
-        <v>12567</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="D76" s="5">
-        <v>40080</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="D77" s="5">
-        <v>21980</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="D78" s="5">
-        <v>29400</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="D79" s="5">
-        <v>32285</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D80" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>